<commit_message>
* InputController 지연 현상 해소. (1 frame 고정)  * Error Type, Table 이름 수정.
</commit_message>
<xml_diff>
--- a/input/Domains/Common/tables/CommonTable.xlsx
+++ b/input/Domains/Common/tables/CommonTable.xlsx
@@ -7,7 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="COMPLEX_POLICY" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="ERROR_CLIENT" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ERROR_COMMON" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="ERROR_SERVER" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
@@ -669,7 +669,6 @@
         </is>
       </c>
     </row>
-    <row r="4"/>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
@@ -1399,6 +1398,78 @@
       <c r="C65" t="inlineStr">
         <is>
           <t>Purchase store failed</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>LOGIN_SYNC_CANCELLED</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Sync cancelled</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>LOGIN_SYNC_SLOT_LIST_FAILED</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Sync failed while listing slots</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>LOGIN_SYNC_LOAD_LOCAL_FAILED</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Sync failed while loading local data</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>LOGIN_SYNC_LOAD_CLOUD_FAILED</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Sync failed while loading cloud data</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>LOGIN_SYNC_SAVE_LOCAL_FAILED</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Sync failed while saving local data</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>LOGIN_SYNC_SAVE_CLOUD_FAILED</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Sync failed while saving cloud data</t>
         </is>
       </c>
     </row>
@@ -1441,7 +1512,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>enum:ErrorServerType</t>
+          <t>enum:ServerErrorType</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1458,10 +1529,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>pk, gen:ErrorServerType, code</t>
-        </is>
-      </c>
-    </row>
+          <t>pk, gen:ServerErrorType, code</t>
+        </is>
+      </c>
+    </row>
+    <row r="4"/>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
* SaveDataManager 보완.  * 스킬 정리 및 리팩토링.
</commit_message>
<xml_diff>
--- a/input/Domains/Common/tables/CommonTable.xlsx
+++ b/input/Domains/Common/tables/CommonTable.xlsx
@@ -616,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
@@ -1482,6 +1482,18 @@
       <c r="C72" t="inlineStr">
         <is>
           <t>Sync failed while resolving conflict</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>SAVEDATA_PAYLOAD_PARSE_FAILED</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Failed to parse save payload json</t>
         </is>
       </c>
     </row>

</xml_diff>